<commit_message>
hmm tjaeh bum bum
huhej vilde dyr
</commit_message>
<xml_diff>
--- a/tabel/delanalyse1_noegletalniveau1og5.xlsx
+++ b/tabel/delanalyse1_noegletalniveau1og5.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bubba\Dropbox\Speciale\Emil_Soeren\latexopgave\tabel\excel_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bubba\Dropbox\Speciale\Emil_Soeren\latexopgave\tabel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14280"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14280" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="delanalyse1_noegletalniveau1og5" sheetId="1" r:id="rId1"/>
+    <sheet name="delanalyse1_" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
   <si>
     <t>Niveau</t>
   </si>
@@ -236,6 +238,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -271,6 +290,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -425,13 +461,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="13.25" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -558,4 +594,109 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="5">
+        <v>271</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.68</v>
+      </c>
+      <c r="D3" s="5">
+        <v>12</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0.67600000000000005</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0.97399999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="7">
+        <v>51</v>
+      </c>
+      <c r="C4" s="8">
+        <v>0.79</v>
+      </c>
+      <c r="D4" s="7">
+        <v>10</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0.80300000000000005</v>
+      </c>
+      <c r="F4" s="8">
+        <v>0.51800000000000002</v>
+      </c>
+      <c r="G4" s="8">
+        <v>0.95799999999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>